<commit_message>
Added access to data in responses because it was missing from changing fetch to axios
</commit_message>
<xml_diff>
--- a/fax planning.xlsx
+++ b/fax planning.xlsx
@@ -490,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -523,9 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,6 +532,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +968,7 @@
       <c r="G6" s="1">
         <v>43995</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <v>43996</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -975,7 +976,7 @@
       </c>
     </row>
     <row r="7" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="32">
         <v>43997</v>
       </c>
       <c r="C7" s="11">
@@ -1455,37 +1456,37 @@
       <c r="H31" s="22"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="L35" t="s">
@@ -1970,11 +1971,11 @@
       <c r="C86" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D86" s="28" t="s">
+      <c r="D86" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="25">
@@ -1988,29 +1989,24 @@
       <c r="C88" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D88" s="28" t="s">
+      <c r="D88" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="J21:N21"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="P21:V21"/>
-    <mergeCell ref="P22:V22"/>
-    <mergeCell ref="P23:V23"/>
-    <mergeCell ref="P24:V24"/>
-    <mergeCell ref="P25:V25"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="D86:F86"/>
     <mergeCell ref="P20:V20"/>
     <mergeCell ref="J15:N15"/>
     <mergeCell ref="J16:N16"/>
@@ -2022,22 +2018,27 @@
     <mergeCell ref="P17:V17"/>
     <mergeCell ref="P18:V18"/>
     <mergeCell ref="P19:V19"/>
+    <mergeCell ref="P21:V21"/>
+    <mergeCell ref="P22:V22"/>
+    <mergeCell ref="P23:V23"/>
+    <mergeCell ref="P24:V24"/>
+    <mergeCell ref="P25:V25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="J21:N21"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B25:H25"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="J23:N23"/>
     <mergeCell ref="J24:N24"/>
     <mergeCell ref="B21:H21"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="D86:F86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>